<commit_message>
Changed Arum's part and Excel
Changed Arum's part and Excel
</commit_message>
<xml_diff>
--- a/No Free Lunch.xlsx
+++ b/No Free Lunch.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lily/Documents/3. Exploratory Data Analysis and Visualization/3. HW/HW1/Git/Project_final/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32580" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Ian Johnson</t>
   </si>
@@ -90,12 +92,12 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,14 +110,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -135,66 +131,6 @@
       </top>
       <bottom style="thin">
         <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -234,7 +170,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -244,32 +180,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -345,6 +266,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1455,320 +1381,87 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV23"/>
+  <dimension ref="A1:IO8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="12" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1"/>
+    <col min="2" max="249" width="12" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:2" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="20.5" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+    <row r="7" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="20.5" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8" t="s">
+    <row r="8" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>